<commit_message>
edit ekspor user and cctv
</commit_message>
<xml_diff>
--- a/cctv_export.xlsx
+++ b/cctv_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ip Addres</t>
+          <t>Ip Address</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -453,136 +453,816 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Parkiran Motor</t>
+          <t>Ruang AKP</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.10.201</t>
+          <t>192.168.1.199</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pos Satpam</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>strinssssg</t>
+          <t xml:space="preserve">Ruang Perawat Kaber </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.10.207</t>
+          <t>192.168.1.101</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pos Satpam</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>Ruang Praktik</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.10.100</t>
+          <t>192.168.1.202</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Pos Satpam</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Parkiran Mobil</t>
+          <t>Lorong AKP</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.10.202</t>
+          <t>192.168.1.201</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pos Satpam</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lorong Ct-Scan</t>
+          <t>Lorong Lotus</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.10.159</t>
+          <t>192.168.1.208</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pos security depan</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>testttt</t>
+          <t>Ruang Istirahat</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>192.168.10.206</t>
+          <t>192.168.1.100</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Pos security depan</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lorong gudan farmasi hd</t>
+          <t>Ruang Obat Gudang Farmasi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>192.168.10.101</t>
+          <t>192.168.1.102</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Pos security depan</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Pos Satya 123</t>
+          <t>Gudang farmasi</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>192.168.101.20</t>
+          <t>192.168.1.103</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pos security depan</t>
+          <t>Owner Akupuntur (Ns Lotus)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Lorong Rosalina</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>192.168.10.201</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lorong NS1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>192.168.10.202</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lorong VVIP A</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>192.168.10.153</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Lorong VVIP B</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>192.168.10.154</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Lorong Tulip kls 2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>192.168.10.118</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mushola</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>192.168.10.192</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Lorong Mushola Tangga kanan</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>192.168.10.188</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>IPC Kasir Inap</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>192.168.10.107</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Lorong Umum</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>192.168.10.157</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Gazebo Kantin Teratai</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>192.168.10.116</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Aula Barat</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>192.168.10.211</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CSSD-OK-KU</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>192.168.10.212</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Depo_OK</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>192.168.10.214</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Poli Paru</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>192.168.10.196</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Server IT</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>192.168.10.164</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Pos security Alamanda</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>TPS</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>192.168.10.105</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Depan ICU</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>192.168.10.187</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Pos Pintu Masuk lorong depan RSCH</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>192.168.10.193</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ruang Farmasi RJ</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>192.168.10.213</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Pintu Masuk Farmasi RJ</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>192.168.10.221</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Lorong IGD,TPP,Pos Securty Depan</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>192.168.10.109</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Tunggu Poli</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>192.168.10.225</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Lorong Poli Anak 1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>192.168.10.167</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ruang Tunggu Pendaftaran</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>192.168.10.226</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Gazebo Perin</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>192.168.10.162</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lorong Perin Kaber </t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>192.168.10.161</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Rekam Medis</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>192.168.10.165</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Lorong Radiologi</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>192.168.10.163</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Lorong ruang Teratai D E</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>192.168.10.156</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Lorong Gudang Farmasi HD</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>192.168.10.101</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Lorong CT-Scan</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>192.168.10.159</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Pos security depan</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Selasar Lorong Keluar Teratai D dan E gazebo</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>192.168.10.104</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Nurse Station 2 Teratai</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Selasar Nurse Teratai pintu keluar</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>192.168.10.102</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Nurse Station 2 Teratai</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Ruang NS 1</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>192.168.1.153</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Nurse Station 1 Rosalina</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Kasir Inap</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>192.168.1.107</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Nurse Station 1 Rosalina</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Selasar Barat VVIP</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>192.168.1.187</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Nurse Station 1 Rosalina</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Lorong Mushola</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>192.168.1.188</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Nurse Station 1 Rosalina</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Mati</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>192.168.1.118</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Nurse Station 1 Rosalina</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ruang Bayi </t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>192.168.10.103</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Perawat Perinatologi</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ruang Perawat </t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>192.168.10.160</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Perawat Perinatologi</t>
         </is>
       </c>
     </row>

</xml_diff>